<commit_message>
Replace timer with await in add and remove subscriber functions
</commit_message>
<xml_diff>
--- a/Solution Design Document.xlsx
+++ b/Solution Design Document.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\olorin4\web-dev\campaign-monitor-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACED9B5F-BB49-4A51-87A1-F1BD40E573DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4BCDBD-957F-49B0-B3EE-3F69C6EDE9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>event name</t>
   </si>
@@ -95,6 +108,12 @@
   </si>
   <si>
     <t>focus_duration</t>
+  </si>
+  <si>
+    <t>device_type</t>
+  </si>
+  <si>
+    <t>user_agent</t>
   </si>
 </sst>
 </file>
@@ -377,7 +396,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="19.8" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -463,6 +482,12 @@
       </c>
       <c r="B5" s="4" t="s">
         <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>22</v>

</xml_diff>